<commit_message>
Leave one out analysis and creation of non-spiro rule
</commit_message>
<xml_diff>
--- a/01_DA_fasta/Cyclase-Library.xlsx
+++ b/01_DA_fasta/Cyclase-Library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/sw17073_bristol_ac_uk/Documents/BrisEngBio/Cyclase-15/Alignment_tree/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/saedwi_dtu_dk/Documents/02_Collab/Diels-Alderase/01_DA_fasta/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="89" documentId="8_{0A226D89-BC0A-A045-9400-86C0800BF4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F15EE6FA-89AB-9140-ABFB-765A4006AAD4}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="760" windowWidth="26280" windowHeight="13680" activeTab="1" xr2:uid="{0CE77C3E-2A21-40F0-A67D-29CF56D545FB}"/>
+    <workbookView xWindow="28680" yWindow="-1395" windowWidth="29040" windowHeight="15720" xr2:uid="{0CE77C3E-2A21-40F0-A67D-29CF56D545FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cyclase Lib" sheetId="1" r:id="rId1"/>
@@ -1527,7 +1527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1594,12 +1594,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1615,11 +1609,14 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2600,8 +2597,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1352550" y="45732701"/>
-          <a:ext cx="2438475" cy="1417874"/>
+          <a:off x="1238250" y="44243626"/>
+          <a:ext cx="2276550" cy="1354374"/>
           <a:chOff x="2242481" y="3104671"/>
           <a:chExt cx="2247975" cy="1355167"/>
         </a:xfrm>
@@ -3062,8 +3059,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1333500" y="64147700"/>
-          <a:ext cx="2261301" cy="2025499"/>
+          <a:off x="1219200" y="61922025"/>
+          <a:ext cx="2096201" cy="1933424"/>
           <a:chOff x="2439984" y="3595838"/>
           <a:chExt cx="2070801" cy="1936599"/>
         </a:xfrm>
@@ -4999,10 +4996,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A99292A-62F2-3544-B44B-F5F1180F84DF}" name="Table1" displayName="Table1" ref="A1:C48" totalsRowShown="0">
   <autoFilter ref="A1:C48" xr:uid="{3A99292A-62F2-3544-B44B-F5F1180F84DF}"/>
@@ -5019,9 +5012,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5059,7 +5052,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5165,7 +5158,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5307,7 +5300,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5317,31 +5310,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE186BB-C08F-4CA6-BE51-617A0B780AE1}">
   <dimension ref="A2:Q45"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C26" sqref="B26:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="15" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:17" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
@@ -5376,7 +5369,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5411,7 +5404,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -5446,7 +5439,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -5479,7 +5472,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -5514,7 +5507,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -5549,7 +5542,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -5587,7 +5580,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -5625,7 +5618,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5663,7 +5656,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -5698,7 +5691,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -5736,7 +5729,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -5771,7 +5764,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -5806,7 +5799,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -5848,7 +5841,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -5888,7 +5881,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -5927,7 +5920,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -5966,7 +5959,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -6008,7 +6001,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -6050,7 +6043,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>109</v>
       </c>
@@ -6086,7 +6079,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>114</v>
       </c>
@@ -6125,7 +6118,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>120</v>
       </c>
@@ -6167,7 +6160,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -6203,7 +6196,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -6239,7 +6232,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>136</v>
       </c>
@@ -6278,7 +6271,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>141</v>
       </c>
@@ -6313,7 +6306,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>147</v>
       </c>
@@ -6354,7 +6347,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="33" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -6389,7 +6382,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>159</v>
       </c>
@@ -6427,7 +6420,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>166</v>
       </c>
@@ -6462,7 +6455,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>171</v>
       </c>
@@ -6497,7 +6490,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>176</v>
       </c>
@@ -6535,7 +6528,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>183</v>
       </c>
@@ -6573,7 +6566,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -6611,7 +6604,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>196</v>
       </c>
@@ -6649,7 +6642,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>202</v>
       </c>
@@ -6684,7 +6677,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>208</v>
       </c>
@@ -6719,7 +6712,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>214</v>
       </c>
@@ -6757,7 +6750,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>221</v>
       </c>
@@ -6795,7 +6788,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>228</v>
       </c>
@@ -6830,7 +6823,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>234</v>
       </c>
@@ -6865,7 +6858,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>240</v>
       </c>
@@ -6903,7 +6896,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>321</v>
       </c>
@@ -6923,7 +6916,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>322</v>
       </c>
@@ -6963,7 +6956,7 @@
     <hyperlink ref="M30" r:id="rId18" xr:uid="{3CE534FC-CEA5-4939-A934-AA8E58894473}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6971,16 +6964,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E27C6E-8928-9445-8DFB-C62429B4803A}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6991,17 +6984,17 @@
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="35" t="s">
         <v>335</v>
       </c>
       <c r="B2" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="40" t="s">
         <v>335</v>
       </c>
-      <c r="D2" s="40" t="str">
+      <c r="D2" s="38" t="str">
         <f>IF(ISNUMBER(MATCH(C2,A:A,0)), "Present", "Absent")</f>
         <v>Present</v>
       </c>
@@ -7009,690 +7002,690 @@
         <v>347</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="16" t="s">
         <v>337</v>
       </c>
       <c r="B3" t="s">
         <v>340</v>
       </c>
-      <c r="D3" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C4,A:A,0)), "Present", "Absent")</f>
+      <c r="D3" s="38" t="str">
+        <f t="shared" ref="D3:D32" si="0">IF(ISNUMBER(MATCH(C4,A:A,0)), "Present", "Absent")</f>
         <v>Present</v>
       </c>
       <c r="G3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C5,A:A,0)), "Present", "Absent")</f>
+      <c r="D4" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="35" t="s">
         <v>336</v>
       </c>
       <c r="B5" t="s">
         <v>341</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="39" t="s">
         <v>336</v>
       </c>
-      <c r="D5" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C6,A:A,0)), "Present", "Absent")</f>
+      <c r="D5" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>184</v>
       </c>
       <c r="B6" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="D6" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C7,A:A,0)), "Present", "Absent")</f>
+      <c r="D6" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="18" t="s">
         <v>142</v>
       </c>
       <c r="B7" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C8,A:A,0)), "Present", "Absent")</f>
+      <c r="D7" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C9,A:A,0)), "Present", "Absent")</f>
+      <c r="D8" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="17" t="s">
         <v>75</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C10,A:A,0)), "Present", "Absent")</f>
+      <c r="D9" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="17" t="s">
         <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C11,A:A,0)), "Present", "Absent")</f>
+      <c r="D10" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="17" t="s">
         <v>86</v>
       </c>
       <c r="B11" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C12,A:A,0)), "Present", "Absent")</f>
+      <c r="D11" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="17" t="s">
         <v>92</v>
       </c>
       <c r="B12" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C13,A:A,0)), "Present", "Absent")</f>
+      <c r="D12" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="17" t="s">
         <v>104</v>
       </c>
       <c r="B13" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C14,A:A,0)), "Present", "Absent")</f>
+      <c r="D13" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="17" t="s">
         <v>115</v>
       </c>
       <c r="B14" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C15,A:A,0)), "Present", "Absent")</f>
+      <c r="D14" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="17" t="s">
         <v>121</v>
       </c>
       <c r="B15" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C16,A:A,0)), "Present", "Absent")</f>
+      <c r="D15" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="17" t="s">
         <v>127</v>
       </c>
       <c r="B16" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C17,A:A,0)), "Present", "Absent")</f>
+      <c r="D16" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B17" t="s">
         <v>135</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="D17" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C18,A:A,0)), "Present", "Absent")</f>
+      <c r="D17" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="17" t="s">
         <v>137</v>
       </c>
       <c r="B18" t="s">
         <v>140</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C19,A:A,0)), "Present", "Absent")</f>
+      <c r="D18" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="16" t="s">
         <v>167</v>
       </c>
       <c r="B19" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="D19" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C20,A:A,0)), "Present", "Absent")</f>
+      <c r="D19" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="16" t="s">
         <v>229</v>
       </c>
       <c r="B20" t="s">
         <v>233</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="D20" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C21,A:A,0)), "Present", "Absent")</f>
+      <c r="D20" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="16" t="s">
         <v>209</v>
       </c>
       <c r="B21" t="s">
         <v>213</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="D21" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C22,A:A,0)), "Present", "Absent")</f>
+      <c r="D21" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Absent</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="16" t="s">
         <v>309</v>
       </c>
       <c r="B22" t="s">
         <v>201</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="43" t="s">
         <v>345</v>
       </c>
-      <c r="D22" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C23,A:A,0)), "Present", "Absent")</f>
+      <c r="D22" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="35" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C24,A:A,0)), "Present", "Absent")</f>
+      <c r="D23" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="16" t="s">
         <v>222</v>
       </c>
       <c r="B24" t="s">
         <v>227</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="D24" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C25,A:A,0)), "Present", "Absent")</f>
+      <c r="D24" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="35" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C26,A:A,0)), "Present", "Absent")</f>
+      <c r="D25" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Absent</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="34" t="s">
         <v>203</v>
       </c>
       <c r="B26" t="s">
         <v>207</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="39" t="s">
         <v>311</v>
       </c>
-      <c r="D26" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C27,A:A,0)), "Present", "Absent")</f>
+      <c r="D26" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="35" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C28,A:A,0)), "Present", "Absent")</f>
+      <c r="D27" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="16" t="s">
         <v>154</v>
       </c>
       <c r="B28" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="D28" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C29,A:A,0)), "Present", "Absent")</f>
+      <c r="D28" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="17" t="s">
         <v>98</v>
       </c>
       <c r="B29" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C30,A:A,0)), "Present", "Absent")</f>
+      <c r="D29" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="17" t="s">
         <v>110</v>
       </c>
       <c r="B30" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C31,A:A,0)), "Present", "Absent")</f>
+      <c r="D30" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="16" t="s">
         <v>241</v>
       </c>
       <c r="B31" t="s">
         <v>246</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="D31" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C32,A:A,0)), "Present", "Absent")</f>
+      <c r="D31" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="16" t="s">
         <v>215</v>
       </c>
       <c r="B32" t="s">
         <v>220</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="D32" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C33,A:A,0)), "Present", "Absent")</f>
+      <c r="D32" s="38" t="str">
+        <f t="shared" si="0"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="16" t="s">
         <v>190</v>
       </c>
       <c r="B33" t="s">
         <v>195</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="39" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C35,A:A,0)), "Present", "Absent")</f>
+      <c r="D33" s="38" t="str">
+        <f t="shared" ref="D33:D39" si="1">IF(ISNUMBER(MATCH(C35,A:A,0)), "Present", "Absent")</f>
         <v>Present</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="16" t="s">
         <v>338</v>
       </c>
       <c r="B34" t="s">
         <v>342</v>
       </c>
-      <c r="D34" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C36,A:A,0)), "Present", "Absent")</f>
+      <c r="D34" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="16" t="s">
         <v>235</v>
       </c>
       <c r="B35" t="s">
         <v>239</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="C35" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="D35" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C37,A:A,0)), "Present", "Absent")</f>
+      <c r="D35" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="16" t="s">
         <v>148</v>
       </c>
       <c r="B36" t="s">
         <v>152</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C38,A:A,0)), "Present", "Absent")</f>
+      <c r="D36" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="35" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C39,A:A,0)), "Present", "Absent")</f>
+      <c r="D37" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="35" t="s">
         <v>42</v>
       </c>
       <c r="B38" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C40,A:A,0)), "Present", "Absent")</f>
+      <c r="D38" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="35" t="s">
         <v>48</v>
       </c>
       <c r="B39" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="40" t="str">
-        <f>IF(ISNUMBER(MATCH(C41,A:A,0)), "Present", "Absent")</f>
+      <c r="D39" s="38" t="str">
+        <f t="shared" si="1"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="16" t="s">
         <v>319</v>
       </c>
       <c r="B40" t="s">
         <v>343</v>
       </c>
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="D40" s="40" t="str">
+      <c r="D40" s="38" t="str">
         <f>IF(ISNUMBER(MATCH(#REF!,A:A,0)), "Present", "Absent")</f>
         <v>Absent</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="16" t="s">
         <v>177</v>
       </c>
       <c r="B41" t="s">
         <v>182</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="D41" s="40" t="str">
+      <c r="D41" s="38" t="str">
         <f>IF(ISNUMBER(MATCH(C42,A:A,0)), "Present", "Absent")</f>
         <v>Present</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="16" t="s">
         <v>160</v>
       </c>
       <c r="B42" t="s">
         <v>165</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="D42" s="40" t="str">
+      <c r="D42" s="38" t="str">
         <f>IF(ISNUMBER(MATCH(C43,A:A,0)), "Present", "Absent")</f>
         <v>Present</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="35" t="s">
         <v>52</v>
       </c>
       <c r="B43" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C43" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D43" s="40" t="str">
+      <c r="D43" s="38" t="str">
         <f>IF(ISNUMBER(MATCH(C44,A:A,0)), "Present", "Absent")</f>
         <v>Present</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="16" t="s">
         <v>320</v>
       </c>
       <c r="B44" t="s">
         <v>344</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="39" t="s">
         <v>320</v>
       </c>
-      <c r="D44" s="40" t="str">
+      <c r="D44" s="38" t="str">
         <f>IF(ISNUMBER(MATCH(#REF!,A:A,0)), "Present", "Absent")</f>
         <v>Absent</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="36" t="s">
         <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="40" t="str">
-        <f t="shared" ref="D3:D48" si="0">IF(ISNUMBER(MATCH(C45,A:A,0)), "Present", "Absent")</f>
+      <c r="D45" s="38" t="str">
+        <f t="shared" ref="D45:D48" si="2">IF(ISNUMBER(MATCH(C45,A:A,0)), "Present", "Absent")</f>
         <v>Present</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="16" t="s">
         <v>172</v>
       </c>
       <c r="B46" t="s">
         <v>175</v>
       </c>
-      <c r="C46" s="44" t="s">
+      <c r="C46" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="D46" s="40" t="str">
-        <f t="shared" si="0"/>
+      <c r="D46" s="38" t="str">
+        <f t="shared" si="2"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="37" t="s">
         <v>69</v>
       </c>
       <c r="B47" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="41" t="s">
+      <c r="C47" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="40" t="str">
-        <f t="shared" si="0"/>
+      <c r="D47" s="38" t="str">
+        <f t="shared" si="2"/>
         <v>Present</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B48" t="s">
         <v>67</v>
       </c>
-      <c r="C48" s="45" t="s">
+      <c r="C48" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="D48" s="40" t="str">
-        <f t="shared" si="0"/>
+      <c r="D48" s="38" t="str">
+        <f t="shared" si="2"/>
         <v>Present</v>
       </c>
     </row>
@@ -7746,21 +7739,21 @@
       <selection activeCell="R74" sqref="R74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" style="19"/>
+    <col min="2" max="2" width="8.6328125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="45"/>
       <c r="C1" s="28" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="23" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="23" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
@@ -7771,7 +7764,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -7779,7 +7772,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="23" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="23" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>19</v>
       </c>
@@ -7790,7 +7783,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A31" s="23" t="s">
         <v>24</v>
       </c>
@@ -7804,7 +7797,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -7812,7 +7805,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -7820,7 +7813,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="23" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" s="23" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A59" s="23" t="s">
         <v>41</v>
       </c>
@@ -7831,7 +7824,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>47</v>
       </c>
@@ -7839,7 +7832,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>51</v>
       </c>
@@ -7847,7 +7840,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A88" s="23" t="s">
         <v>57</v>
       </c>
@@ -7861,19 +7854,19 @@
         <v>286</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="23"/>
       <c r="B89" s="26"/>
       <c r="C89" s="24"/>
       <c r="D89" s="24"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="23"/>
       <c r="B90" s="26"/>
       <c r="C90" s="24"/>
       <c r="D90" s="24"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -7881,7 +7874,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A107" s="23" t="s">
         <v>68</v>
       </c>
@@ -7899,7 +7892,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>301</v>
       </c>
@@ -7907,7 +7900,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="114" spans="1:6" s="23" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" s="23" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A114" s="23" t="s">
         <v>141</v>
       </c>
@@ -7918,7 +7911,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>147</v>
       </c>
@@ -7926,7 +7919,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>153</v>
       </c>
@@ -7934,17 +7927,17 @@
         <v>154</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F137" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F138" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>159</v>
       </c>
@@ -7952,7 +7945,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>166</v>
       </c>
@@ -7960,7 +7953,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>171</v>
       </c>
@@ -7968,7 +7961,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>176</v>
       </c>
@@ -7976,7 +7969,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>183</v>
       </c>
@@ -7984,7 +7977,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>189</v>
       </c>
@@ -7992,7 +7985,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>196</v>
       </c>
@@ -8000,7 +7993,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="238" spans="1:6" s="23" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" s="23" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A238" s="23" t="s">
         <v>202</v>
       </c>
@@ -8011,7 +8004,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>208</v>
       </c>
@@ -8019,7 +8012,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>214</v>
       </c>
@@ -8027,7 +8020,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>221</v>
       </c>
@@ -8035,7 +8028,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>228</v>
       </c>
@@ -8043,7 +8036,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>234</v>
       </c>
@@ -8051,12 +8044,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J309" s="33" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="310" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>240</v>
       </c>
@@ -8070,12 +8063,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.35">
       <c r="L311" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>321</v>
       </c>
@@ -8088,8 +8081,8 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8101,9 +8094,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:14" ht="128" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>141</v>
       </c>
@@ -8120,12 +8113,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="J4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -8142,7 +8135,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>171</v>
       </c>
@@ -8156,7 +8149,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="23" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" s="23" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A38" s="23" t="s">
         <v>202</v>
       </c>
@@ -8167,7 +8160,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -8181,7 +8174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="23" t="s">
         <v>41</v>
       </c>
@@ -8192,7 +8185,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -8214,9 +8207,9 @@
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>221</v>
       </c>
@@ -8232,10 +8225,23 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="1ee89e71-04cd-405e-9ca3-99e020c1694d" ContentTypeId="0x0101" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Keyword xmlns="44a56295-c29e-4898-8136-a54736c65b82" xsi:nil="true"/>
+    <Descriptions xmlns="44a56295-c29e-4898-8136-a54736c65b82" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001A7323DF848F0046B9FF89A5C08C45D6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1d8b1641ba26d66fe313da2ffc92a3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="44a56295-c29e-4898-8136-a54736c65b82" xmlns:ns4="f78785e1-c54a-437f-a5a6-c2f4110c0915" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0151976f3dca5f88d1b7aa134c0cb267" ns3:_="" ns4:_="">
     <xsd:import namespace="44a56295-c29e-4898-8136-a54736c65b82"/>
@@ -8434,33 +8440,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Keyword xmlns="44a56295-c29e-4898-8136-a54736c65b82" xsi:nil="true"/>
-    <Descriptions xmlns="44a56295-c29e-4898-8136-a54736c65b82" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="1ee89e71-04cd-405e-9ca3-99e020c1694d" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CB72A0-B0C5-4285-A358-3C0FFE06E339}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{529BFE51-F626-401F-A58D-6951A47898F8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC1CCB39-6521-4C6C-BCCF-1A78FD66A226}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="44a56295-c29e-4898-8136-a54736c65b82"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f78785e1-c54a-437f-a5a6-c2f4110c0915"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F9E746-E1DE-4DBC-9AC4-B75867369862}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8479,27 +8489,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC1CCB39-6521-4C6C-BCCF-1A78FD66A226}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07CB72A0-B0C5-4285-A358-3C0FFE06E339}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="44a56295-c29e-4898-8136-a54736c65b82"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f78785e1-c54a-437f-a5a6-c2f4110c0915"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{529BFE51-F626-401F-A58D-6951A47898F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>